<commit_message>
Formatos de celda y autorelleno
</commit_message>
<xml_diff>
--- a/excel-basico/1-fundamentos-y-navegacion-en-excel.xlsx
+++ b/excel-basico/1-fundamentos-y-navegacion-en-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\excel-learn\excel-basico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3260F2B5-463F-498F-B9C5-C1E5E1A2536C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF79839-9CB6-422E-9D97-587DE467CDB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28453,7 +28453,7 @@
   <dimension ref="E1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>